<commit_message>
Fixed the issue of adding codewordset functionality
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Testcodeword1</t>
   </si>
@@ -36,6 +36,30 @@
   </si>
   <si>
     <t>Testcodeword4</t>
+  </si>
+  <si>
+    <t>Testcodeword5</t>
+  </si>
+  <si>
+    <t>Testcodeword6</t>
+  </si>
+  <si>
+    <t>Testcodeword7</t>
+  </si>
+  <si>
+    <t>Testcodeword8</t>
+  </si>
+  <si>
+    <t>Testcodeword9</t>
+  </si>
+  <si>
+    <t>Testcodeword10</t>
+  </si>
+  <si>
+    <t>Testcodeword11</t>
+  </si>
+  <si>
+    <t>Testcodeword12</t>
   </si>
 </sst>
 </file>
@@ -353,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,6 +408,46 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Hint for creating codewordset
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s530473\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s530473\Desktop\GDP-2\Seperate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Testcodeword1</t>
   </si>
@@ -54,12 +54,6 @@
   </si>
   <si>
     <t>Testcodeword10</t>
-  </si>
-  <si>
-    <t>Testcodeword11</t>
-  </si>
-  <si>
-    <t>Testcodeword12</t>
   </si>
 </sst>
 </file>
@@ -377,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A14" sqref="A11:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,16 +432,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>